<commit_message>
Agregando plantilla de repsuesto, modificando data
</commit_message>
<xml_diff>
--- a/PLANTILLA.xlsx
+++ b/PLANTILLA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uzzie\Documents\Jale\automatizador-crediflexi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA293DB9-3C82-4975-9051-4200746F58B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B8927AF-69AA-4E58-9D30-F029DFCD53E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -544,7 +544,7 @@
     <cellStyle name="Normal 18" xfId="3" xr:uid="{2A504B10-7F54-4E2D-B0E4-83871B6AC25A}"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="116">
+  <dxfs count="69">
     <dxf>
       <alignment vertical="top"/>
     </dxf>
@@ -905,286 +905,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000066"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000066"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000066"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000066"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment vertical="top"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="top"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="top"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="top"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000066"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000066"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000066"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" wrapText="1"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000066"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" wrapText="1"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000066"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000066"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -3788,10 +3508,10 @@
   <dimension ref="A4:S15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="8" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="8" topLeftCell="F9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="H23" sqref="H23"/>
+      <selection pane="bottomRight" activeCell="N11" sqref="N11:N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3938,10 +3658,6 @@
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
-      <c r="H9" s="14">
-        <f>IFERROR(D9/E9,0)</f>
-        <v>0</v>
-      </c>
       <c r="I9" s="16"/>
       <c r="J9" s="13" t="s">
         <v>87</v>
@@ -3960,7 +3676,7 @@
       <c r="F10" s="26"/>
       <c r="G10" s="26"/>
       <c r="H10" s="14">
-        <f>IFERROR(D10/E10,0)</f>
+        <f>IFERROR(D9/E9,0)</f>
         <v>0</v>
       </c>
       <c r="I10" s="16"/>
@@ -3972,26 +3688,30 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="H11" s="14">
-        <f t="shared" ref="H11:H13" si="0">IFERROR(D11/E11,0)</f>
+        <f>IFERROR(D10/E10,0)</f>
         <v>0</v>
       </c>
       <c r="I11" s="16"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="H12" s="14">
-        <f t="shared" si="0"/>
+        <f>IFERROR(D11/E11,0)</f>
         <v>0</v>
       </c>
       <c r="I12" s="16"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="H13" s="14">
-        <f t="shared" si="0"/>
+        <f>IFERROR(D12/E12,0)</f>
         <v>0</v>
       </c>
       <c r="I13" s="16"/>
     </row>
     <row r="14" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H14" s="14">
+        <f>IFERROR(D13/E13,0)</f>
+        <v>0</v>
+      </c>
       <c r="I14" s="16"/>
     </row>
     <row r="15" spans="1:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>